<commit_message>
Backup QR Scanner data - 2025-12-16T08:16:35.089Z - Cache Bust: 1765872995089
</commit_message>
<xml_diff>
--- a/log_history/Y5_B2526_Neurology_scanner1765872189076_b4df4d3060ee5a11a9fb4fe245eb3c4dfaf42a930352ff25ac8e7238642d95b9.xlsx
+++ b/log_history/Y5_B2526_Neurology_scanner1765872189076_b4df4d3060ee5a11a9fb4fe245eb3c4dfaf42a930352ff25ac8e7238642d95b9.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="Session" sheetId="1" r:id="rId1"/>
+    <sheet name="Neurology" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F36"/>
+  <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1122,9 +1122,49 @@
         <v>emp17.farah.a.youssef@gmail.com</v>
       </c>
     </row>
+    <row r="37">
+      <c r="A37" t="str">
+        <v>190333</v>
+      </c>
+      <c r="B37" t="str">
+        <v>Neurology</v>
+      </c>
+      <c r="C37" t="str">
+        <v>16/12/2025</v>
+      </c>
+      <c r="D37" t="str">
+        <v>10:13:46</v>
+      </c>
+      <c r="E37" t="str">
+        <v>Manual</v>
+      </c>
+      <c r="F37" t="str">
+        <v>emp17.farah.a.youssef@gmail.com</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="str">
+        <v>191007</v>
+      </c>
+      <c r="B38" t="str">
+        <v>Neurology</v>
+      </c>
+      <c r="C38" t="str">
+        <v>16/12/2025</v>
+      </c>
+      <c r="D38" t="str">
+        <v>10:16:24</v>
+      </c>
+      <c r="E38" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F38" t="str">
+        <v>emp17.farah.a.youssef@gmail.com</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F36"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F38"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update edited session - 2025-12-16T08:16:42.765Z - Cache Bust ID: 1765873002765ro5onuzfq
</commit_message>
<xml_diff>
--- a/log_history/Y5_B2526_Neurology_scanner1765872189076_b4df4d3060ee5a11a9fb4fe245eb3c4dfaf42a930352ff25ac8e7238642d95b9.xlsx
+++ b/log_history/Y5_B2526_Neurology_scanner1765872189076_b4df4d3060ee5a11a9fb4fe245eb3c4dfaf42a930352ff25ac8e7238642d95b9.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="Neurology" sheetId="1" r:id="rId1"/>
+    <sheet name="Session" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F38"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1122,49 +1122,9 @@
         <v>emp17.farah.a.youssef@gmail.com</v>
       </c>
     </row>
-    <row r="37">
-      <c r="A37" t="str">
-        <v>190333</v>
-      </c>
-      <c r="B37" t="str">
-        <v>Neurology</v>
-      </c>
-      <c r="C37" t="str">
-        <v>16/12/2025</v>
-      </c>
-      <c r="D37" t="str">
-        <v>10:13:46</v>
-      </c>
-      <c r="E37" t="str">
-        <v>Manual</v>
-      </c>
-      <c r="F37" t="str">
-        <v>emp17.farah.a.youssef@gmail.com</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="str">
-        <v>191007</v>
-      </c>
-      <c r="B38" t="str">
-        <v>Neurology</v>
-      </c>
-      <c r="C38" t="str">
-        <v>16/12/2025</v>
-      </c>
-      <c r="D38" t="str">
-        <v>10:16:24</v>
-      </c>
-      <c r="E38" t="str">
-        <v>Scan</v>
-      </c>
-      <c r="F38" t="str">
-        <v>emp17.farah.a.youssef@gmail.com</v>
-      </c>
-    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F38"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F36"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Backup QR Scanner data - 2025-12-16T08:50:25.160Z - Cache Bust: 1765875025160
</commit_message>
<xml_diff>
--- a/log_history/Y5_B2526_Neurology_scanner1765872189076_b4df4d3060ee5a11a9fb4fe245eb3c4dfaf42a930352ff25ac8e7238642d95b9.xlsx
+++ b/log_history/Y5_B2526_Neurology_scanner1765872189076_b4df4d3060ee5a11a9fb4fe245eb3c4dfaf42a930352ff25ac8e7238642d95b9.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="Session" sheetId="1" r:id="rId1"/>
+    <sheet name="Neurology" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F36"/>
+  <dimension ref="A1:F39"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1122,9 +1122,69 @@
         <v>emp17.farah.a.youssef@gmail.com</v>
       </c>
     </row>
+    <row r="37">
+      <c r="A37" t="str">
+        <v>190333</v>
+      </c>
+      <c r="B37" t="str">
+        <v>Neurology</v>
+      </c>
+      <c r="C37" t="str">
+        <v>16/12/2025</v>
+      </c>
+      <c r="D37" t="str">
+        <v>10:13:46</v>
+      </c>
+      <c r="E37" t="str">
+        <v>Manual</v>
+      </c>
+      <c r="F37" t="str">
+        <v>emp17.farah.a.youssef@gmail.com</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="str">
+        <v>191007</v>
+      </c>
+      <c r="B38" t="str">
+        <v>Neurology</v>
+      </c>
+      <c r="C38" t="str">
+        <v>16/12/2025</v>
+      </c>
+      <c r="D38" t="str">
+        <v>10:16:24</v>
+      </c>
+      <c r="E38" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F38" t="str">
+        <v>emp17.farah.a.youssef@gmail.com</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="str">
+        <v>202051</v>
+      </c>
+      <c r="B39" t="str">
+        <v>Neurology</v>
+      </c>
+      <c r="C39" t="str">
+        <v>16/12/2025</v>
+      </c>
+      <c r="D39" t="str">
+        <v>10:48:43</v>
+      </c>
+      <c r="E39" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F39" t="str">
+        <v>emp17.farah.a.youssef@gmail.com</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F36"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F39"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update edited session - 2025-12-16T08:50:32.817Z - Cache Bust ID: 1765875032817a50pgwmo5
</commit_message>
<xml_diff>
--- a/log_history/Y5_B2526_Neurology_scanner1765872189076_b4df4d3060ee5a11a9fb4fe245eb3c4dfaf42a930352ff25ac8e7238642d95b9.xlsx
+++ b/log_history/Y5_B2526_Neurology_scanner1765872189076_b4df4d3060ee5a11a9fb4fe245eb3c4dfaf42a930352ff25ac8e7238642d95b9.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="Neurology" sheetId="1" r:id="rId1"/>
+    <sheet name="Session" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F39"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1122,69 +1122,9 @@
         <v>emp17.farah.a.youssef@gmail.com</v>
       </c>
     </row>
-    <row r="37">
-      <c r="A37" t="str">
-        <v>190333</v>
-      </c>
-      <c r="B37" t="str">
-        <v>Neurology</v>
-      </c>
-      <c r="C37" t="str">
-        <v>16/12/2025</v>
-      </c>
-      <c r="D37" t="str">
-        <v>10:13:46</v>
-      </c>
-      <c r="E37" t="str">
-        <v>Manual</v>
-      </c>
-      <c r="F37" t="str">
-        <v>emp17.farah.a.youssef@gmail.com</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="str">
-        <v>191007</v>
-      </c>
-      <c r="B38" t="str">
-        <v>Neurology</v>
-      </c>
-      <c r="C38" t="str">
-        <v>16/12/2025</v>
-      </c>
-      <c r="D38" t="str">
-        <v>10:16:24</v>
-      </c>
-      <c r="E38" t="str">
-        <v>Scan</v>
-      </c>
-      <c r="F38" t="str">
-        <v>emp17.farah.a.youssef@gmail.com</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="str">
-        <v>202051</v>
-      </c>
-      <c r="B39" t="str">
-        <v>Neurology</v>
-      </c>
-      <c r="C39" t="str">
-        <v>16/12/2025</v>
-      </c>
-      <c r="D39" t="str">
-        <v>10:48:43</v>
-      </c>
-      <c r="E39" t="str">
-        <v>Scan</v>
-      </c>
-      <c r="F39" t="str">
-        <v>emp17.farah.a.youssef@gmail.com</v>
-      </c>
-    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F39"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F36"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Backup QR Scanner data - 2025-12-16T08:52:45.572Z - Cache Bust: 1765875165572
</commit_message>
<xml_diff>
--- a/log_history/Y5_B2526_Neurology_scanner1765872189076_b4df4d3060ee5a11a9fb4fe245eb3c4dfaf42a930352ff25ac8e7238642d95b9.xlsx
+++ b/log_history/Y5_B2526_Neurology_scanner1765872189076_b4df4d3060ee5a11a9fb4fe245eb3c4dfaf42a930352ff25ac8e7238642d95b9.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="Session" sheetId="1" r:id="rId1"/>
+    <sheet name="Neurology" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F36"/>
+  <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1122,9 +1122,89 @@
         <v>emp17.farah.a.youssef@gmail.com</v>
       </c>
     </row>
+    <row r="37">
+      <c r="A37" t="str">
+        <v>190333</v>
+      </c>
+      <c r="B37" t="str">
+        <v>Neurology</v>
+      </c>
+      <c r="C37" t="str">
+        <v>16/12/2025</v>
+      </c>
+      <c r="D37" t="str">
+        <v>10:13:46</v>
+      </c>
+      <c r="E37" t="str">
+        <v>Manual</v>
+      </c>
+      <c r="F37" t="str">
+        <v>emp17.farah.a.youssef@gmail.com</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="str">
+        <v>191007</v>
+      </c>
+      <c r="B38" t="str">
+        <v>Neurology</v>
+      </c>
+      <c r="C38" t="str">
+        <v>16/12/2025</v>
+      </c>
+      <c r="D38" t="str">
+        <v>10:16:24</v>
+      </c>
+      <c r="E38" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F38" t="str">
+        <v>emp17.farah.a.youssef@gmail.com</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="str">
+        <v>202051</v>
+      </c>
+      <c r="B39" t="str">
+        <v>Neurology</v>
+      </c>
+      <c r="C39" t="str">
+        <v>16/12/2025</v>
+      </c>
+      <c r="D39" t="str">
+        <v>10:48:43</v>
+      </c>
+      <c r="E39" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F39" t="str">
+        <v>emp17.farah.a.youssef@gmail.com</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="str">
+        <v>210728</v>
+      </c>
+      <c r="B40" t="str">
+        <v>Neurology</v>
+      </c>
+      <c r="C40" t="str">
+        <v>16/12/2025</v>
+      </c>
+      <c r="D40" t="str">
+        <v>10:52:36</v>
+      </c>
+      <c r="E40" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F40" t="str">
+        <v>emp17.farah.a.youssef@gmail.com</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F36"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F40"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update edited session - 2025-12-16T08:52:58.378Z - Cache Bust ID: 17658751783783t3r3v3v2
</commit_message>
<xml_diff>
--- a/log_history/Y5_B2526_Neurology_scanner1765872189076_b4df4d3060ee5a11a9fb4fe245eb3c4dfaf42a930352ff25ac8e7238642d95b9.xlsx
+++ b/log_history/Y5_B2526_Neurology_scanner1765872189076_b4df4d3060ee5a11a9fb4fe245eb3c4dfaf42a930352ff25ac8e7238642d95b9.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="Neurology" sheetId="1" r:id="rId1"/>
+    <sheet name="Session" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F40"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1122,89 +1122,9 @@
         <v>emp17.farah.a.youssef@gmail.com</v>
       </c>
     </row>
-    <row r="37">
-      <c r="A37" t="str">
-        <v>190333</v>
-      </c>
-      <c r="B37" t="str">
-        <v>Neurology</v>
-      </c>
-      <c r="C37" t="str">
-        <v>16/12/2025</v>
-      </c>
-      <c r="D37" t="str">
-        <v>10:13:46</v>
-      </c>
-      <c r="E37" t="str">
-        <v>Manual</v>
-      </c>
-      <c r="F37" t="str">
-        <v>emp17.farah.a.youssef@gmail.com</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="str">
-        <v>191007</v>
-      </c>
-      <c r="B38" t="str">
-        <v>Neurology</v>
-      </c>
-      <c r="C38" t="str">
-        <v>16/12/2025</v>
-      </c>
-      <c r="D38" t="str">
-        <v>10:16:24</v>
-      </c>
-      <c r="E38" t="str">
-        <v>Scan</v>
-      </c>
-      <c r="F38" t="str">
-        <v>emp17.farah.a.youssef@gmail.com</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="str">
-        <v>202051</v>
-      </c>
-      <c r="B39" t="str">
-        <v>Neurology</v>
-      </c>
-      <c r="C39" t="str">
-        <v>16/12/2025</v>
-      </c>
-      <c r="D39" t="str">
-        <v>10:48:43</v>
-      </c>
-      <c r="E39" t="str">
-        <v>Scan</v>
-      </c>
-      <c r="F39" t="str">
-        <v>emp17.farah.a.youssef@gmail.com</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="str">
-        <v>210728</v>
-      </c>
-      <c r="B40" t="str">
-        <v>Neurology</v>
-      </c>
-      <c r="C40" t="str">
-        <v>16/12/2025</v>
-      </c>
-      <c r="D40" t="str">
-        <v>10:52:36</v>
-      </c>
-      <c r="E40" t="str">
-        <v>Scan</v>
-      </c>
-      <c r="F40" t="str">
-        <v>emp17.farah.a.youssef@gmail.com</v>
-      </c>
-    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F40"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F36"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update edited session - 2025-12-16T09:10:59.587Z - Cache Bust ID: 1765876259587oxu2uyc07
</commit_message>
<xml_diff>
--- a/log_history/Y5_B2526_Neurology_scanner1765872189076_b4df4d3060ee5a11a9fb4fe245eb3c4dfaf42a930352ff25ac8e7238642d95b9.xlsx
+++ b/log_history/Y5_B2526_Neurology_scanner1765872189076_b4df4d3060ee5a11a9fb4fe245eb3c4dfaf42a930352ff25ac8e7238642d95b9.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="Neurology" sheetId="1" r:id="rId1"/>
+    <sheet name="Session" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F36"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1122,9 +1122,109 @@
         <v>emp17.farah.a.youssef@gmail.com</v>
       </c>
     </row>
+    <row r="37">
+      <c r="A37" t="str">
+        <v>190333</v>
+      </c>
+      <c r="B37" t="str">
+        <v>Neurology</v>
+      </c>
+      <c r="C37" t="str">
+        <v>16/12/2025</v>
+      </c>
+      <c r="D37" t="str">
+        <v>10:13:46</v>
+      </c>
+      <c r="E37" t="str">
+        <v>Manual</v>
+      </c>
+      <c r="F37" t="str">
+        <v>emp17.farah.a.youssef@gmail.com</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="str">
+        <v>191007</v>
+      </c>
+      <c r="B38" t="str">
+        <v>Neurology</v>
+      </c>
+      <c r="C38" t="str">
+        <v>16/12/2025</v>
+      </c>
+      <c r="D38" t="str">
+        <v>10:16:24</v>
+      </c>
+      <c r="E38" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F38" t="str">
+        <v>emp17.farah.a.youssef@gmail.com</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="str">
+        <v>202051</v>
+      </c>
+      <c r="B39" t="str">
+        <v>Neurology</v>
+      </c>
+      <c r="C39" t="str">
+        <v>16/12/2025</v>
+      </c>
+      <c r="D39" t="str">
+        <v>10:48:43</v>
+      </c>
+      <c r="E39" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F39" t="str">
+        <v>emp17.farah.a.youssef@gmail.com</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="str">
+        <v>210728</v>
+      </c>
+      <c r="B40" t="str">
+        <v>Neurology</v>
+      </c>
+      <c r="C40" t="str">
+        <v>16/12/2025</v>
+      </c>
+      <c r="D40" t="str">
+        <v>10:52:36</v>
+      </c>
+      <c r="E40" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F40" t="str">
+        <v>emp17.farah.a.youssef@gmail.com</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="str">
+        <v>212075</v>
+      </c>
+      <c r="B41" t="str">
+        <v>Neurology</v>
+      </c>
+      <c r="C41" t="str">
+        <v>16/12/2025</v>
+      </c>
+      <c r="D41" t="str">
+        <v>11:10:38</v>
+      </c>
+      <c r="E41" t="str">
+        <v>Manual</v>
+      </c>
+      <c r="F41" t="str">
+        <v>emp17.farah.a.youssef@gmail.com</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F36"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F41"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Backup QR Scanner data - 2025-12-16T09:14:22.527Z - Cache Bust: 1765876462527
</commit_message>
<xml_diff>
--- a/log_history/Y5_B2526_Neurology_scanner1765872189076_b4df4d3060ee5a11a9fb4fe245eb3c4dfaf42a930352ff25ac8e7238642d95b9.xlsx
+++ b/log_history/Y5_B2526_Neurology_scanner1765872189076_b4df4d3060ee5a11a9fb4fe245eb3c4dfaf42a930352ff25ac8e7238642d95b9.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="Session" sheetId="1" r:id="rId1"/>
+    <sheet name="Neurology" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F41"/>
+  <dimension ref="A1:F42"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1222,9 +1222,29 @@
         <v>emp17.farah.a.youssef@gmail.com</v>
       </c>
     </row>
+    <row r="42">
+      <c r="A42" t="str">
+        <v>212024</v>
+      </c>
+      <c r="B42" t="str">
+        <v>Neurology</v>
+      </c>
+      <c r="C42" t="str">
+        <v>16/12/2025</v>
+      </c>
+      <c r="D42" t="str">
+        <v>11:12:55</v>
+      </c>
+      <c r="E42" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F42" t="str">
+        <v>emp17.farah.a.youssef@gmail.com</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F41"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F42"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update edited session - 2025-12-16T09:14:30.837Z - Cache Bust ID: 1765876470837cy5c58ylo
</commit_message>
<xml_diff>
--- a/log_history/Y5_B2526_Neurology_scanner1765872189076_b4df4d3060ee5a11a9fb4fe245eb3c4dfaf42a930352ff25ac8e7238642d95b9.xlsx
+++ b/log_history/Y5_B2526_Neurology_scanner1765872189076_b4df4d3060ee5a11a9fb4fe245eb3c4dfaf42a930352ff25ac8e7238642d95b9.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="Neurology" sheetId="1" r:id="rId1"/>
+    <sheet name="Session" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F42"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1222,29 +1222,9 @@
         <v>emp17.farah.a.youssef@gmail.com</v>
       </c>
     </row>
-    <row r="42">
-      <c r="A42" t="str">
-        <v>212024</v>
-      </c>
-      <c r="B42" t="str">
-        <v>Neurology</v>
-      </c>
-      <c r="C42" t="str">
-        <v>16/12/2025</v>
-      </c>
-      <c r="D42" t="str">
-        <v>11:12:55</v>
-      </c>
-      <c r="E42" t="str">
-        <v>Scan</v>
-      </c>
-      <c r="F42" t="str">
-        <v>emp17.farah.a.youssef@gmail.com</v>
-      </c>
-    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F42"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F41"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update edited session - 2025-12-16T11:26:40.427Z - Cache Bust ID: 17658844004272lsz12cxw
</commit_message>
<xml_diff>
--- a/log_history/Y5_B2526_Neurology_scanner1765872189076_b4df4d3060ee5a11a9fb4fe245eb3c4dfaf42a930352ff25ac8e7238642d95b9.xlsx
+++ b/log_history/Y5_B2526_Neurology_scanner1765872189076_b4df4d3060ee5a11a9fb4fe245eb3c4dfaf42a930352ff25ac8e7238642d95b9.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="Neurology" sheetId="1" r:id="rId1"/>
+    <sheet name="Session" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F41"/>
+  <dimension ref="A1:F42"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1222,9 +1222,29 @@
         <v>emp17.farah.a.youssef@gmail.com</v>
       </c>
     </row>
+    <row r="42">
+      <c r="A42" t="str">
+        <v>212024</v>
+      </c>
+      <c r="B42" t="str">
+        <v>Neurology</v>
+      </c>
+      <c r="C42" t="str">
+        <v>16/12/2025</v>
+      </c>
+      <c r="D42" t="str">
+        <v>11:12:55</v>
+      </c>
+      <c r="E42" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F42" t="str">
+        <v>emp17.farah.a.youssef@gmail.com</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F41"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F42"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Backup QR Scanner data - 2025-12-20T10:30:56.253Z - Cache Bust: 1766226656253
</commit_message>
<xml_diff>
--- a/log_history/Y5_B2526_Neurology_scanner1765872189076_b4df4d3060ee5a11a9fb4fe245eb3c4dfaf42a930352ff25ac8e7238642d95b9.xlsx
+++ b/log_history/Y5_B2526_Neurology_scanner1765872189076_b4df4d3060ee5a11a9fb4fe245eb3c4dfaf42a930352ff25ac8e7238642d95b9.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F42"/>
+  <dimension ref="A1:F43"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1242,9 +1242,29 @@
         <v>emp17.farah.a.youssef@gmail.com</v>
       </c>
     </row>
+    <row r="43">
+      <c r="A43" t="str">
+        <v>202048</v>
+      </c>
+      <c r="B43" t="str">
+        <v>Neurology</v>
+      </c>
+      <c r="C43" t="str">
+        <v>16/12/2025</v>
+      </c>
+      <c r="D43" t="str">
+        <v>12:50:15</v>
+      </c>
+      <c r="E43" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F43" t="str">
+        <v>emp17.farah.a.youssef@gmail.com</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F42"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F43"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>